<commit_message>
Update turn righr and add configable camera
</commit_message>
<xml_diff>
--- a/resource/cmd.xlsx
+++ b/resource/cmd.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">STT</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">fl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">turn</t>
   </si>
 </sst>
 </file>
@@ -162,10 +165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -289,6 +292,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>